<commit_message>
Resultados de testes executados até então.
</commit_message>
<xml_diff>
--- a/artigo/src/test/resources/AllClassifierTests 20170728-211603.xlsx
+++ b/artigo/src/test/resources/AllClassifierTests 20170728-211603.xlsx
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P11"/>
+  <dimension ref="B1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,6 +1007,171 @@
       <c r="P11" s="4">
         <v>0.84440000000000004</v>
       </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>